<commit_message>
Implemented Profile section validation
</commit_message>
<xml_diff>
--- a/src/test/resource/test-data/orangehrmautomation.xlsx
+++ b/src/test/resource/test-data/orangehrmautomation.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>url</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Support</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ossupport@orangehrm.com </t>
   </si>
   <si>
     <t>Changepassword</t>
@@ -88,7 +91,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -97,6 +100,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -378,15 +384,18 @@
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated about section validation
</commit_message>
<xml_diff>
--- a/src/test/resource/test-data/orangehrmautomation.xlsx
+++ b/src/test/resource/test-data/orangehrmautomation.xlsx
@@ -41,7 +41,7 @@
     <t>About</t>
   </si>
   <si>
-    <t>OrangeHRM</t>
+    <t>OrangeHRM OS 5.7</t>
   </si>
   <si>
     <t>Support</t>
@@ -60,7 +60,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -71,10 +71,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,7 +94,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -347,10 +343,7 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-  </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>